<commit_message>
fix null data in dashboard
</commit_message>
<xml_diff>
--- a/scriptDatabase/fomat_quarantined_person.xlsx
+++ b/scriptDatabase/fomat_quarantined_person.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\UIT\Nam 3\HKI\PP OOP\Project\QuanLyKhuCachLy\scriptDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0785A273-348F-4F7F-BD4C-F1CC5C2BEB85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE6BEA2-3B44-4CBA-BC6F-EF29EADB7863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{53B6D07A-B72C-4875-A261-E7F84EEB7438}"/>
+    <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{53B6D07A-B72C-4875-A261-E7F84EEB7438}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="47">
   <si>
     <t>STT</t>
   </si>
@@ -78,28 +78,103 @@
     <t>Phòng</t>
   </si>
   <si>
-    <t>ho va ten 1</t>
-  </si>
-  <si>
     <t>Nam</t>
   </si>
   <si>
-    <t>thon , xa , huyen, tinh</t>
-  </si>
-  <si>
-    <t>VietNam</t>
-  </si>
-  <si>
     <t>ho,sốt,đau họng</t>
   </si>
   <si>
-    <t>ho va ten 2</t>
-  </si>
-  <si>
     <t>Nữ</t>
   </si>
   <si>
     <t>khó thở</t>
+  </si>
+  <si>
+    <t>Trương Kim Lâm</t>
+  </si>
+  <si>
+    <t>Dương Hiển Thế</t>
+  </si>
+  <si>
+    <t>Huỳnh Trọng Phục</t>
+  </si>
+  <si>
+    <t>Trần Lê Thanh Tùng</t>
+  </si>
+  <si>
+    <t>Trương Kim Phục</t>
+  </si>
+  <si>
+    <t>Trương Kim Thế</t>
+  </si>
+  <si>
+    <t>Trần Lê Thanh Thế</t>
+  </si>
+  <si>
+    <t>Trương Thanh Phục</t>
+  </si>
+  <si>
+    <t>Huỳnh Trọng Lâm</t>
+  </si>
+  <si>
+    <t>Dương Hiển Tùng</t>
+  </si>
+  <si>
+    <t>Dương Lê Thanh Thế</t>
+  </si>
+  <si>
+    <t>Huỳnh Trọng Thế</t>
+  </si>
+  <si>
+    <t>Dương Hiển Trọng Phục</t>
+  </si>
+  <si>
+    <t>Trương Kim Tùng</t>
+  </si>
+  <si>
+    <t>60 Cây Keo, Hiệp Tân, Tân Phú, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>61 Cây Keo, Hiệp Tân, Tân Phú, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>62 Cây Keo, Hiệp Tân, Tân Phú, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>63 Cây Keo, Hiệp Tân, Tân Phú, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>64 Cây Keo, Hiệp Tân, Tân Phú, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>65 Cây Keo, Hiệp Tân, Tân Phú, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>66 Cây Keo, Hiệp Tân, Tân Phú, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>67 Cây Keo, Hiệp Tân, Tân Phú, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>68 Cây Keo, Hiệp Tân, Tân Phú, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>69 Cây Keo, Hiệp Tân, Tân Phú, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>70 Cây Keo, Hiệp Tân, Tân Phú, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>71 Cây Keo, Hiệp Tân, Tân Phú, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>72 Cây Keo, Hiệp Tân, Tân Phú, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>73 Cây Keo, Hiệp Tân, Tân Phú, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Việt Nam</t>
   </si>
 </sst>
 </file>
@@ -140,7 +215,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -156,7 +231,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -452,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3CD999E-6D30-4CC0-AB9A-DF9962F9583E}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,6 +538,7 @@
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -514,40 +590,37 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1">
-        <v>44292</v>
+        <v>37107</v>
       </c>
       <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2">
+        <v>79201017231</v>
+      </c>
+      <c r="H2">
+        <v>69</v>
+      </c>
+      <c r="I2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2">
+        <v>84357255117</v>
+      </c>
+      <c r="K2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2">
-        <v>19922</v>
-      </c>
-      <c r="H2">
-        <v>3113</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2">
-        <v>220032</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
       <c r="M2" s="1">
-        <v>44257</v>
+        <v>44516</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -558,37 +631,490 @@
         <v>19</v>
       </c>
       <c r="C3" s="1">
-        <v>36527</v>
+        <v>38931</v>
       </c>
       <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3">
+        <v>79201017232</v>
+      </c>
+      <c r="H3">
+        <v>70</v>
+      </c>
+      <c r="I3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3">
+        <v>84906012839</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="1">
+        <v>44516</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C4" s="1">
+        <v>36444</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3">
-        <v>21991</v>
-      </c>
-      <c r="H3">
-        <v>1313415</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3">
-        <v>2288932</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4">
+        <v>79201017283</v>
+      </c>
+      <c r="H4">
+        <v>71</v>
+      </c>
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4">
+        <v>84035725515</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="1">
+        <v>44519</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1">
-        <v>44258</v>
+      <c r="C5" s="1">
+        <v>36881</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5">
+        <v>79201016283</v>
+      </c>
+      <c r="H5">
+        <v>72</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5">
+        <v>84035725516</v>
+      </c>
+      <c r="K5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="1">
+        <v>44519</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1">
+        <v>32050</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6">
+        <v>79201027283</v>
+      </c>
+      <c r="H6">
+        <v>73</v>
+      </c>
+      <c r="I6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6">
+        <v>84035725517</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="1">
+        <v>44520</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1">
+        <v>32011</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7">
+        <v>79201087283</v>
+      </c>
+      <c r="H7">
+        <v>74</v>
+      </c>
+      <c r="I7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7">
+        <v>84035725518</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="1">
+        <v>44520</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1">
+        <v>32012</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8">
+        <v>79201029283</v>
+      </c>
+      <c r="H8">
+        <v>75</v>
+      </c>
+      <c r="I8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8">
+        <v>84035725519</v>
+      </c>
+      <c r="K8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="1">
+        <v>44520</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1">
+        <v>32013</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9">
+        <v>79201098283</v>
+      </c>
+      <c r="H9">
+        <v>76</v>
+      </c>
+      <c r="I9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9">
+        <v>84035725520</v>
+      </c>
+      <c r="K9" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" s="1">
+        <v>44520</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1">
+        <v>32014</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10">
+        <v>79201018273</v>
+      </c>
+      <c r="H10">
+        <v>77</v>
+      </c>
+      <c r="I10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10">
+        <v>84035725521</v>
+      </c>
+      <c r="K10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="1">
+        <v>44524</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1">
+        <v>32015</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11">
+        <v>79201090283</v>
+      </c>
+      <c r="H11">
+        <v>78</v>
+      </c>
+      <c r="I11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11">
+        <v>84035725522</v>
+      </c>
+      <c r="K11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" s="1">
+        <v>44524</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1">
+        <v>32016</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12">
+        <v>79201017219</v>
+      </c>
+      <c r="H12">
+        <v>79</v>
+      </c>
+      <c r="I12" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12">
+        <v>84035725523</v>
+      </c>
+      <c r="K12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" s="1">
+        <v>44524</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="1">
+        <v>32017</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13">
+        <v>79201017220</v>
+      </c>
+      <c r="H13">
+        <v>80</v>
+      </c>
+      <c r="I13" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13">
+        <v>84035725524</v>
+      </c>
+      <c r="K13" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" s="1">
+        <v>44528</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1">
+        <v>32018</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14">
+        <v>79201017592</v>
+      </c>
+      <c r="H14">
+        <v>81</v>
+      </c>
+      <c r="I14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14">
+        <v>84035725525</v>
+      </c>
+      <c r="K14" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="1">
+        <v>44528</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1">
+        <v>32019</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15">
+        <v>79201018592</v>
+      </c>
+      <c r="H15">
+        <v>82</v>
+      </c>
+      <c r="I15" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15">
+        <v>84035725526</v>
+      </c>
+      <c r="K15" t="s">
+        <v>17</v>
+      </c>
+      <c r="M15" s="1">
+        <v>44529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>